<commit_message>
Commit 2 Issuer Changes
</commit_message>
<xml_diff>
--- a/ENTITYISSUER/src/test/resources/DataSource/Accounts.xlsx
+++ b/ENTITYISSUER/src/test/resources/DataSource/Accounts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guptat3/IdeaProjects/mss-esgc-solutions-test-automation/ENTITYISSUER/src/test/resources/DataSource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82D7984-AE2D-AF4E-A434-6517578BF57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5270D064-2F80-1D44-BB14-905A949EE15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19860" activeTab="3" xr2:uid="{0EF049D3-A00D-B24D-8507-3C49E149D925}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19880" activeTab="2" xr2:uid="{0EF049D3-A00D-B24D-8507-3C49E149D925}"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="UAT" sheetId="3" r:id="rId3"/>
     <sheet name="PROD" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="68">
   <si>
     <t>UserName</t>
   </si>
@@ -213,6 +213,36 @@
   </si>
   <si>
     <t>Littelfuse, Inc.</t>
+  </si>
+  <si>
+    <t>000025275</t>
+  </si>
+  <si>
+    <t>L.B. Foster Co.</t>
+  </si>
+  <si>
+    <t>mesg-platform-testing+metrics1@outlook.com</t>
+  </si>
+  <si>
+    <t>mesg-platform-testing+metrics6@outlook.com</t>
+  </si>
+  <si>
+    <t>UFP Industries, Inc.</t>
+  </si>
+  <si>
+    <t>000100504</t>
+  </si>
+  <si>
+    <t>THE SHYFT GROUP, INC.</t>
+  </si>
+  <si>
+    <t>mesg-platform-issuer-qa+test18@outlook.com</t>
+  </si>
+  <si>
+    <t>Gray Television, Inc.</t>
+  </si>
+  <si>
+    <t>000292337</t>
   </si>
 </sst>
 </file>
@@ -328,7 +358,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -616,7 +646,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -624,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA75EBF-7D9E-AC41-8A41-AFD325DD971D}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -670,23 +700,23 @@
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
+      <c r="B2" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>15</v>
@@ -694,25 +724,25 @@
     </row>
     <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>15</v>
@@ -720,25 +750,25 @@
     </row>
     <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>15</v>
@@ -746,25 +776,25 @@
     </row>
     <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>15</v>
@@ -775,19 +805,19 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>26</v>
@@ -797,55 +827,67 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{279CC46A-0A79-2249-AD4A-09585E4B0FD1}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{DEC91CF3-5B07-8346-834E-667940C41531}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{59F90C52-671A-904B-98BC-B2EFF64075CE}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{F520DCF1-A887-774F-A589-F13D3C34A8BE}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{DCD1DB95-99B5-1F47-BEBC-B7D0EF94B5BA}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{CF868D61-FC14-0645-B7C0-6106E6F1FC64}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{CF2090D1-F2E6-2147-9BB2-EBD89ADF2D10}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{C8DC43F5-3A87-8645-A637-834B8B83653C}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{E77B89A9-4149-DA48-B141-164A446C9CA2}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{8D167FAA-00B4-9648-B914-5EA452973422}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{DC71697E-EA9D-7A4A-BA48-FC4828BF771E}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{04E2EDDB-EC04-964E-99B1-C93D75FECA30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1083,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A406E6F1-7655-CF44-8DBE-2F0D93D1AB54}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1232,7 +1274,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>7</v>
@@ -1241,10 +1283,10 @@
         <v>21</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>26</v>
@@ -1258,7 +1300,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>7</v>
@@ -1267,10 +1309,10 @@
         <v>21</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>26</v>
@@ -1284,7 +1326,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>7</v>
@@ -1293,10 +1335,10 @@
         <v>29</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>26</v>
@@ -1323,8 +1365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E667755A-3D54-2D42-B2CB-137C4645F872}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>